<commit_message>
Basic cisteni dat pridano
</commit_message>
<xml_diff>
--- a/data/Inflace_2000-23.xlsx
+++ b/data/Inflace_2000-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\Hackathon-Game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E07F2A6-8C1C-44D7-887B-AF63A58BE4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D31E5E-CD54-4573-A49C-DDEE18A82965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Úhrn</t>
   </si>
@@ -70,9 +70,6 @@
   <si>
     <t>Ostatní zboží 
 a služby</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Rok</t>
@@ -432,7 +429,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -442,7 +439,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -820,12 +817,8 @@
       <c r="I9">
         <v>0.4</v>
       </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
       <c r="K9">
-        <f>A20</f>
-        <v>2018</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>2.4</v>

</xml_diff>